<commit_message>
Updated LCA process names
</commit_message>
<xml_diff>
--- a/public/lcad-evaluation/assets/data/LCA/Design A/Process contribution A - Amount.XLSX
+++ b/public/lcad-evaluation/assets/data/LCA/Design A/Process contribution A - Amount.XLSX
@@ -3,37 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="XLSReadWriteII" lastEdited="4" lowestEdited="4" rupBuild="4.00.38"/>
   <sheets>
-    <sheet name="Sheet6" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="48">
-  <si>
-    <t>Turning Chamfers 1, 2, 3, 4, 5, 7</t>
-  </si>
-  <si>
-    <t>mg</t>
-  </si>
-  <si>
-    <t>Turning Surface 1</t>
-  </si>
-  <si>
-    <t>Turning Surface 7</t>
-  </si>
-  <si>
-    <t>Turning Top Hole</t>
-  </si>
-  <si>
-    <t>Turning Groove 2</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="47">
+  <si>
+    <t>Turning 11</t>
+  </si>
+  <si>
+    <t>Milling</t>
   </si>
   <si>
     <t>SimaPro 8.5.2.0</t>
   </si>
   <si>
-    <t>Turning Surface 4, Face 4, Bearing Surface 1</t>
+    <t>Turning 13</t>
   </si>
   <si>
     <t>No</t>
@@ -45,6 +33,9 @@
     <t>Exclude infrastructure processes: </t>
   </si>
   <si>
+    <t>Turning 4</t>
+  </si>
+  <si>
     <t>Sort order: </t>
   </si>
   <si>
@@ -54,24 +45,27 @@
     <t>Process contribution</t>
   </si>
   <si>
+    <t>Turning 8</t>
+  </si>
+  <si>
+    <t>Turning 6</t>
+  </si>
+  <si>
     <t>Inventory</t>
   </si>
   <si>
-    <t>Grinding Bearing Surfaces 1, 2</t>
+    <t>Turning 2</t>
   </si>
   <si>
     <t>Results: </t>
   </si>
   <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>Turning Fillets 1, 2, 3, 4, 5, 6, 7, 8, 9</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
+    <t>Turning 10</t>
+  </si>
+  <si>
     <t>Default units: </t>
   </si>
   <si>
@@ -81,19 +75,19 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Turning Groove 1</t>
-  </si>
-  <si>
-    <t>Turning Surface 2, Face 2</t>
-  </si>
-  <si>
-    <t>Turning Chamfer 6</t>
+    <t>Induction Hardening</t>
   </si>
   <si>
     <t>kg</t>
   </si>
   <si>
-    <t>Induction Hardening Bearing Surfaces 1, 2</t>
+    <t>Turning 14</t>
+  </si>
+  <si>
+    <t>Drilling</t>
+  </si>
+  <si>
+    <t>Turning 12</t>
   </si>
   <si>
     <t>Total</t>
@@ -105,7 +99,7 @@
     <t>1 p Screw Pump Shaft (of project Screw Pump Shaft)</t>
   </si>
   <si>
-    <t>Turning Surface 6</t>
+    <t>Yes</t>
   </si>
   <si>
     <t>Exclude long-term emissions: </t>
@@ -117,43 +111,46 @@
     <t>MJ</t>
   </si>
   <si>
-    <t>Turning Surface 5, Face 5, Bearing Surface 2</t>
+    <t>Turning 1</t>
   </si>
   <si>
     <t>ReCiPe 2016 Midpoint (H) V1.00</t>
   </si>
   <si>
-    <t>Milling Keyway</t>
-  </si>
-  <si>
-    <t>Turning Face 3</t>
-  </si>
-  <si>
     <t>Indicator: </t>
   </si>
   <si>
     <t>Date:</t>
   </si>
   <si>
+    <t>Surface Grinding</t>
+  </si>
+  <si>
+    <t>Turning 5</t>
+  </si>
+  <si>
     <t>Product: </t>
   </si>
   <si>
     <t>Calculation: </t>
   </si>
   <si>
+    <t>Turning 3</t>
+  </si>
+  <si>
     <t>Screw Pump Shaft</t>
   </si>
   <si>
-    <t>Drilling Bushing Holes</t>
-  </si>
-  <si>
     <t>Ascending</t>
   </si>
   <si>
+    <t>Turning 7</t>
+  </si>
+  <si>
+    <t>Turning 9</t>
+  </si>
+  <si>
     <t>Process</t>
-  </si>
-  <si>
-    <t>Turning Face 1</t>
   </si>
 </sst>
 </file>
@@ -521,99 +518,99 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1">
-        <v>45572</v>
+        <v>45574</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F1" s="2">
-        <v>0.810479328703704</v>
+        <v>0.919046898148148</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
         <v>46</v>
@@ -621,84 +618,84 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
         <v>46</v>
       </c>
       <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" t="s">
         <v>19</v>
       </c>
-      <c r="D16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" t="s">
-        <v>21</v>
-      </c>
       <c r="G16" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="I16" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="J16" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="K16" t="s">
         <v>38</v>
       </c>
       <c r="L16" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M16" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="N16" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="O16" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="P16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>25</v>
+      </c>
+      <c r="S16" t="s">
         <v>3</v>
       </c>
-      <c r="Q16" t="s">
-        <v>4</v>
-      </c>
-      <c r="R16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S16" t="s">
-        <v>18</v>
-      </c>
       <c r="T16" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="U16" t="s">
+        <v>1</v>
+      </c>
+      <c r="V16" t="s">
+        <v>23</v>
+      </c>
+      <c r="W16" t="s">
         <v>37</v>
       </c>
-      <c r="V16" t="s">
-        <v>25</v>
-      </c>
-      <c r="W16" t="s">
-        <v>15</v>
-      </c>
       <c r="X16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17">
@@ -706,16 +703,16 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E17">
-        <v>91.3200000000506</v>
+        <v>0.09132</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -760,7 +757,7 @@
         <v>0</v>
       </c>
       <c r="T17">
-        <v>91.3200000000506</v>
+        <v>0.09132</v>
       </c>
       <c r="U17">
         <v>0</v>
@@ -780,16 +777,16 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E18">
-        <v>1.00000000000055</v>
+        <v>252</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -843,10 +840,10 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>1.00000000000055</v>
+        <v>0</v>
       </c>
       <c r="X18">
-        <v>0</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19">
@@ -854,16 +851,16 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E19">
-        <v>252</v>
+        <v>0.02224</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -911,7 +908,7 @@
         <v>0</v>
       </c>
       <c r="U19">
-        <v>0</v>
+        <v>0.02224</v>
       </c>
       <c r="V19">
         <v>0</v>
@@ -920,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="X19">
-        <v>252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -928,19 +925,19 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E20">
-        <v>22.2400000000123</v>
+        <v>13.59001</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>13.59001</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -985,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="U20">
-        <v>22.2400000000123</v>
+        <v>0</v>
       </c>
       <c r="V20">
         <v>0</v>
@@ -1002,19 +999,19 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E21">
-        <v>13.59001</v>
+        <v>0.001</v>
       </c>
       <c r="F21">
-        <v>13.59001</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1065,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="W21">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="X21">
         <v>0</v>
@@ -1076,22 +1073,22 @@
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E22">
-        <v>430.000000000316</v>
+        <v>0.70598</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>0.70598</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1136,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="V22">
-        <v>430.000000000316</v>
+        <v>0</v>
       </c>
       <c r="W22">
         <v>0</v>
@@ -1150,16 +1147,16 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E23">
-        <v>2.64000000000146</v>
+        <v>0.07568</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -1192,13 +1189,13 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>0.07568</v>
       </c>
       <c r="Q23">
         <v>0</v>
       </c>
       <c r="R23">
-        <v>2.64000000000146</v>
+        <v>0</v>
       </c>
       <c r="S23">
         <v>0</v>
@@ -1224,22 +1221,22 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E24">
-        <v>705.980000000391</v>
+        <v>0.78442</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>705.980000000391</v>
+        <v>0</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -1269,7 +1266,7 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>0</v>
+        <v>0.78442</v>
       </c>
       <c r="R24">
         <v>0</v>
@@ -1298,16 +1295,16 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E25">
-        <v>2.45273</v>
+        <v>0.00264</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -1325,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>2.45273</v>
+        <v>0</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -1346,7 +1343,7 @@
         <v>0</v>
       </c>
       <c r="R25">
-        <v>0</v>
+        <v>0.00264</v>
       </c>
       <c r="S25">
         <v>0</v>
@@ -1372,16 +1369,16 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E26">
-        <v>4.45000000000247</v>
+        <v>0.00445</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -1423,7 +1420,7 @@
         <v>0</v>
       </c>
       <c r="S26">
-        <v>4.45000000000247</v>
+        <v>0.00445</v>
       </c>
       <c r="T26">
         <v>0</v>
@@ -1449,13 +1446,13 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E27">
-        <v>48.4200000000268</v>
+        <v>0.00043</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -1470,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="J27">
-        <v>48.4200000000268</v>
+        <v>0</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -1506,7 +1503,7 @@
         <v>0</v>
       </c>
       <c r="V27">
-        <v>0</v>
+        <v>0.00043</v>
       </c>
       <c r="W27">
         <v>0</v>
@@ -1520,16 +1517,16 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E28">
-        <v>3.16000000000175</v>
+        <v>0.21985</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -1538,7 +1535,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>0.21985</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1553,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>3.16000000000175</v>
+        <v>0</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -1594,16 +1591,16 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E29">
-        <v>430.000000000316</v>
+        <v>0.00043</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1615,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>430.000000000316</v>
+        <v>0.00043</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -1668,16 +1665,16 @@
         <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E30">
-        <v>219.850000000122</v>
+        <v>0.04842</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1686,13 +1683,13 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <v>219.850000000122</v>
+        <v>0</v>
       </c>
       <c r="I30">
         <v>0</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>0.04842</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -1742,16 +1739,16 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E31">
-        <v>4.8298</v>
+        <v>2.45273</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -1769,10 +1766,10 @@
         <v>0</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>2.45273</v>
       </c>
       <c r="L31">
-        <v>4.8298</v>
+        <v>0</v>
       </c>
       <c r="M31">
         <v>0</v>
@@ -1816,16 +1813,16 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E32">
-        <v>751.840000000417</v>
+        <v>4.8298</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1846,13 +1843,13 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <v>0</v>
+        <v>4.8298</v>
       </c>
       <c r="M32">
         <v>0</v>
       </c>
       <c r="N32">
-        <v>751.840000000417</v>
+        <v>0</v>
       </c>
       <c r="O32">
         <v>0</v>
@@ -1890,16 +1887,16 @@
         <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E33">
-        <v>22.5100000000125</v>
+        <v>0.00316</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1923,13 +1920,13 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <v>0</v>
+        <v>0.00316</v>
       </c>
       <c r="N33">
         <v>0</v>
       </c>
       <c r="O33">
-        <v>22.5100000000125</v>
+        <v>0</v>
       </c>
       <c r="P33">
         <v>0</v>
@@ -1964,16 +1961,16 @@
         <v>18</v>
       </c>
       <c r="B34" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E34">
-        <v>75.6800000000419</v>
+        <v>0.75184</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -2000,13 +1997,13 @@
         <v>0</v>
       </c>
       <c r="N34">
-        <v>0</v>
+        <v>0.75184</v>
       </c>
       <c r="O34">
         <v>0</v>
       </c>
       <c r="P34">
-        <v>75.6800000000419</v>
+        <v>0</v>
       </c>
       <c r="Q34">
         <v>0</v>
@@ -2038,16 +2035,16 @@
         <v>19</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D35" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E35">
-        <v>784.420000000435</v>
+        <v>0.02251</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2077,13 +2074,13 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <v>0</v>
+        <v>0.02251</v>
       </c>
       <c r="P35">
         <v>0</v>
       </c>
       <c r="Q35">
-        <v>784.420000000435</v>
+        <v>0</v>
       </c>
       <c r="R35">
         <v>0</v>

</xml_diff>